<commit_message>
Removed Emergency HTS modality in PEPFAR report
</commit_message>
<xml_diff>
--- a/designs/MER2.2 HTS indicator review, version 2.xlsx
+++ b/designs/MER2.2 HTS indicator review, version 2.xlsx
@@ -5,13 +5,21 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="422" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MER2.2_HTS_TST+HTS_SELF" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="MOH_MER2.2_mapping" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'MOH_MER2.2_mapping'!$D$2:$D$71</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -82,217 +90,217 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3207" uniqueCount="71">
   <si>
-    <t>Indicator</t>
+    <t xml:space="preserve">Indicator</t>
   </si>
   <si>
-    <t>Location</t>
+    <t xml:space="preserve">Location</t>
   </si>
   <si>
-    <t>Mode</t>
+    <t xml:space="preserve">Mode</t>
   </si>
   <si>
-    <t>Sex</t>
+    <t xml:space="preserve">Sex</t>
   </si>
   <si>
-    <t>Age</t>
+    <t xml:space="preserve">Age</t>
   </si>
   <si>
-    <t>Result</t>
+    <t xml:space="preserve">Result</t>
   </si>
   <si>
-    <t>HTS_TST</t>
+    <t xml:space="preserve">HTS_TST</t>
   </si>
   <si>
-    <t>Community</t>
+    <t xml:space="preserve">Community</t>
   </si>
   <si>
-    <t>Index</t>
+    <t xml:space="preserve">Index</t>
   </si>
   <si>
-    <t>MF</t>
+    <t xml:space="preserve">MF</t>
   </si>
   <si>
-    <t>&lt;1</t>
+    <t xml:space="preserve">&lt;1</t>
   </si>
   <si>
-    <t>Neg</t>
+    <t xml:space="preserve">Neg</t>
   </si>
   <si>
-    <t>1-9</t>
+    <t xml:space="preserve">1-9</t>
   </si>
   <si>
-    <t>M</t>
+    <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t>10-14</t>
+    <t xml:space="preserve">10-14</t>
   </si>
   <si>
-    <t>15-19</t>
+    <t xml:space="preserve">15-19</t>
   </si>
   <si>
-    <t>20-24</t>
+    <t xml:space="preserve">20-24</t>
   </si>
   <si>
-    <t>25-29</t>
+    <t xml:space="preserve">25-29</t>
   </si>
   <si>
-    <t>30-34</t>
+    <t xml:space="preserve">30-34</t>
   </si>
   <si>
-    <t>35-39</t>
+    <t xml:space="preserve">35-39</t>
   </si>
   <si>
-    <t>40-49</t>
+    <t xml:space="preserve">40-49</t>
   </si>
   <si>
-    <t>50+</t>
+    <t xml:space="preserve">50+</t>
   </si>
   <si>
-    <t>Pos</t>
+    <t xml:space="preserve">Pos</t>
   </si>
   <si>
-    <t>F</t>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
-    <t>Mobile</t>
+    <t xml:space="preserve">Mobile</t>
   </si>
   <si>
-    <t>VCT</t>
+    <t xml:space="preserve">VCT</t>
   </si>
   <si>
-    <t>Other community platform</t>
+    <t xml:space="preserve">Other community platform</t>
   </si>
   <si>
-    <t>Facility</t>
+    <t xml:space="preserve">Facility</t>
   </si>
   <si>
-    <t>STI</t>
+    <t xml:space="preserve">STI</t>
   </si>
   <si>
-    <t>Inpatient</t>
+    <t xml:space="preserve">Inpatient</t>
   </si>
   <si>
-    <t>Emergency</t>
+    <t xml:space="preserve">Emergency</t>
   </si>
   <si>
-    <t>TB</t>
+    <t xml:space="preserve">TB</t>
   </si>
   <si>
-    <t>VMMC</t>
+    <t xml:space="preserve">VMMC</t>
   </si>
   <si>
-    <t>PMTCT (ANC)</t>
+    <t xml:space="preserve">PMTCT (ANC)</t>
   </si>
   <si>
-    <t>Pediatric</t>
+    <t xml:space="preserve">Pediatric</t>
   </si>
   <si>
-    <t>&lt;5</t>
+    <t xml:space="preserve">&lt;5</t>
   </si>
   <si>
-    <t>Malnutrition</t>
+    <t xml:space="preserve">Malnutrition</t>
   </si>
   <si>
-    <t>Other PITC</t>
+    <t xml:space="preserve">Other PITC</t>
   </si>
   <si>
-    <t>HTS_SELF</t>
+    <t xml:space="preserve">HTS_SELF</t>
   </si>
   <si>
-    <t>Any</t>
+    <t xml:space="preserve">Any</t>
   </si>
   <si>
-    <t>Directly-assisted</t>
+    <t xml:space="preserve">Directly-assisted</t>
   </si>
   <si>
-    <t>Unassisted</t>
+    <t xml:space="preserve">Unassisted</t>
   </si>
   <si>
-    <t>Domain</t>
+    <t xml:space="preserve">Domain</t>
   </si>
   <si>
-    <t>Malawi MOH HTS</t>
+    <t xml:space="preserve">Malawi MOH HTS</t>
   </si>
   <si>
-    <t>PEPFAR MER 2.2</t>
+    <t xml:space="preserve">PEPFAR MER 2.2</t>
   </si>
   <si>
-    <t>Data Source</t>
+    <t xml:space="preserve">Data Source</t>
   </si>
   <si>
-    <t>Register attribute</t>
+    <t xml:space="preserve">Register attribute</t>
   </si>
   <si>
-    <t>Client record</t>
+    <t xml:space="preserve">Client record</t>
   </si>
   <si>
-    <t>Synthesis</t>
+    <t xml:space="preserve">Synthesis</t>
   </si>
   <si>
-    <t>Dimension</t>
+    <t xml:space="preserve">Dimension</t>
   </si>
   <si>
-    <t>Location Type</t>
+    <t xml:space="preserve">Location Type</t>
   </si>
   <si>
-    <t>Service Delivery Point</t>
+    <t xml:space="preserve">Service Delivery Point</t>
   </si>
   <si>
-    <t>Access Type</t>
+    <t xml:space="preserve">Access Type</t>
   </si>
   <si>
-    <t>Partner HIV Status</t>
+    <t xml:space="preserve">Partner HIV Status</t>
   </si>
   <si>
-    <t>Client Age</t>
+    <t xml:space="preserve">Client Age</t>
   </si>
   <si>
-    <t>HTS Setting</t>
+    <t xml:space="preserve">HTS Setting</t>
   </si>
   <si>
-    <t>HTS Modality</t>
+    <t xml:space="preserve">HTS Modality</t>
   </si>
   <si>
-    <t>FRS/Index</t>
+    <t xml:space="preserve">FRS/Index</t>
   </si>
   <si>
-    <t>0-13Y</t>
+    <t xml:space="preserve">0-13Y</t>
   </si>
   <si>
-    <t>Any other</t>
+    <t xml:space="preserve">Any other</t>
   </si>
   <si>
-    <t>Partner Positive</t>
+    <t xml:space="preserve">Partner Positive</t>
   </si>
   <si>
-    <t>PITC</t>
+    <t xml:space="preserve">PITC</t>
   </si>
   <si>
-    <t>VCT/Other</t>
+    <t xml:space="preserve">VCT/Other</t>
   </si>
   <si>
-    <t>Other</t>
+    <t xml:space="preserve">Other</t>
   </si>
   <si>
-    <t>Health Facility</t>
+    <t xml:space="preserve">Health Facility</t>
   </si>
   <si>
-    <t>ANC</t>
+    <t xml:space="preserve">ANC</t>
   </si>
   <si>
-    <t>0-4Y</t>
+    <t xml:space="preserve">0-4Y</t>
   </si>
   <si>
-    <t>5Y+</t>
+    <t xml:space="preserve">5Y+</t>
   </si>
   <si>
-    <t>Maternity</t>
+    <t xml:space="preserve">Maternity</t>
   </si>
   <si>
-    <t>OPD</t>
+    <t xml:space="preserve">OPD</t>
   </si>
   <si>
-    <t>Stand-alone HTS Facility</t>
+    <t xml:space="preserve">Stand-alone HTS Facility</t>
   </si>
 </sst>
 </file>
@@ -300,7 +308,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="10">
@@ -370,7 +378,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +395,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -437,7 +451,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -470,6 +484,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -478,8 +496,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Bad" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Bad" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -544,6 +562,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -551,19 +573,19 @@
   </sheetPr>
   <dimension ref="A1:F452"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M31" activeCellId="0" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1457489878543"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2793522267206"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.71255060728745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9619,30 +9641,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G76" activeCellId="0" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1457489878542"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8542510121458"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.7125506072875"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.5748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -9683,7 +9705,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>49</v>
       </c>
@@ -9709,7 +9731,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
@@ -9732,7 +9754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>7</v>
       </c>
@@ -9755,7 +9777,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>7</v>
       </c>
@@ -9801,7 +9823,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>7</v>
       </c>
@@ -9824,7 +9846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>7</v>
       </c>
@@ -9847,7 +9869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>7</v>
       </c>
@@ -9870,7 +9892,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>7</v>
       </c>
@@ -9916,7 +9938,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>7</v>
       </c>
@@ -9939,7 +9961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>64</v>
       </c>
@@ -9962,7 +9984,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>64</v>
       </c>
@@ -9985,7 +10007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>64</v>
       </c>
@@ -10031,7 +10053,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>64</v>
       </c>
@@ -10054,7 +10076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>64</v>
       </c>
@@ -10077,7 +10099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>64</v>
       </c>
@@ -10100,7 +10122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>64</v>
       </c>
@@ -10146,7 +10168,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>64</v>
       </c>
@@ -10169,7 +10191,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>64</v>
       </c>
@@ -10192,7 +10214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
         <v>64</v>
       </c>
@@ -10215,7 +10237,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>64</v>
       </c>
@@ -10284,7 +10306,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
         <v>64</v>
       </c>
@@ -10307,7 +10329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>64</v>
       </c>
@@ -10330,7 +10352,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
         <v>64</v>
       </c>
@@ -10353,7 +10375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>64</v>
       </c>
@@ -10376,7 +10398,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>64</v>
       </c>
@@ -10422,7 +10444,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
         <v>64</v>
       </c>
@@ -10445,7 +10467,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>64</v>
       </c>
@@ -10468,7 +10490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
         <v>64</v>
       </c>
@@ -10491,7 +10513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
         <v>64</v>
       </c>
@@ -10510,11 +10532,11 @@
       <c r="G38" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="H38" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H38" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
         <v>64</v>
       </c>
@@ -10537,7 +10559,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>64</v>
       </c>
@@ -10560,7 +10582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
         <v>64</v>
       </c>
@@ -10583,7 +10605,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>64</v>
       </c>
@@ -10629,7 +10651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>64</v>
       </c>
@@ -10652,7 +10674,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>64</v>
       </c>
@@ -10675,7 +10697,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>64</v>
       </c>
@@ -10698,7 +10720,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
         <v>64</v>
       </c>
@@ -10767,7 +10789,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>64</v>
       </c>
@@ -10790,7 +10812,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
         <v>64</v>
       </c>
@@ -10813,7 +10835,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
         <v>64</v>
       </c>
@@ -10836,7 +10858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
         <v>64</v>
       </c>
@@ -10859,7 +10881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>64</v>
       </c>
@@ -10905,7 +10927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
         <v>64</v>
       </c>
@@ -10928,7 +10950,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
         <v>64</v>
       </c>
@@ -10951,7 +10973,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
         <v>64</v>
       </c>
@@ -10974,7 +10996,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
         <v>64</v>
       </c>
@@ -11020,7 +11042,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
         <v>64</v>
       </c>
@@ -11043,7 +11065,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
         <v>64</v>
       </c>
@@ -11066,7 +11088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
         <v>64</v>
       </c>
@@ -11089,7 +11111,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
         <v>64</v>
       </c>
@@ -11135,7 +11157,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
         <v>64</v>
       </c>
@@ -11158,7 +11180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
         <v>70</v>
       </c>
@@ -11181,7 +11203,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
         <v>70</v>
       </c>
@@ -11204,7 +11226,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
         <v>70</v>
       </c>
@@ -11250,7 +11272,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
         <v>70</v>
       </c>
@@ -11274,6 +11296,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="D2:D71">
+    <filterColumn colId="0">
+      <customFilters and="true">
+        <customFilter operator="equal" val="PITC"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:H1"/>
@@ -11285,6 +11314,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified MER2.2 definition file and data mapping for PEPFAR reporting to fix some mapping issues
</commit_message>
<xml_diff>
--- a/designs/MER2.2 HTS indicator review, version 2.xlsx
+++ b/designs/MER2.2 HTS indicator review, version 2.xlsx
@@ -5,13 +5,18 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="422" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MER2.2_HTS_TST+HTS_SELF" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="MOH_MER2.2_mapping" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -49,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H39" authorId="0">
+    <comment ref="I41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -80,219 +85,219 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3207" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3309" uniqueCount="71">
   <si>
-    <t>Indicator</t>
+    <t xml:space="preserve">Indicator</t>
   </si>
   <si>
-    <t>Location</t>
+    <t xml:space="preserve">Location</t>
   </si>
   <si>
-    <t>Mode</t>
+    <t xml:space="preserve">Mode</t>
   </si>
   <si>
-    <t>Sex</t>
+    <t xml:space="preserve">Sex</t>
   </si>
   <si>
-    <t>Age</t>
+    <t xml:space="preserve">Age</t>
   </si>
   <si>
-    <t>Result</t>
+    <t xml:space="preserve">Result</t>
   </si>
   <si>
-    <t>HTS_TST</t>
+    <t xml:space="preserve">HTS_TST</t>
   </si>
   <si>
-    <t>Community</t>
+    <t xml:space="preserve">Community</t>
   </si>
   <si>
-    <t>Index</t>
+    <t xml:space="preserve">Index</t>
   </si>
   <si>
-    <t>MF</t>
+    <t xml:space="preserve">MF</t>
   </si>
   <si>
-    <t>&lt;1</t>
+    <t xml:space="preserve">&lt;1</t>
   </si>
   <si>
-    <t>Neg</t>
+    <t xml:space="preserve">Neg</t>
   </si>
   <si>
-    <t>1-9</t>
+    <t xml:space="preserve">1-9</t>
   </si>
   <si>
-    <t>M</t>
+    <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t>10-14</t>
+    <t xml:space="preserve">10-14</t>
   </si>
   <si>
-    <t>15-19</t>
+    <t xml:space="preserve">15-19</t>
   </si>
   <si>
-    <t>20-24</t>
+    <t xml:space="preserve">20-24</t>
   </si>
   <si>
-    <t>25-29</t>
+    <t xml:space="preserve">25-29</t>
   </si>
   <si>
-    <t>30-34</t>
+    <t xml:space="preserve">30-34</t>
   </si>
   <si>
-    <t>35-39</t>
+    <t xml:space="preserve">35-39</t>
   </si>
   <si>
-    <t>40-49</t>
+    <t xml:space="preserve">40-49</t>
   </si>
   <si>
-    <t>50+</t>
+    <t xml:space="preserve">50+</t>
   </si>
   <si>
-    <t>Pos</t>
+    <t xml:space="preserve">Pos</t>
   </si>
   <si>
-    <t>F</t>
+    <t xml:space="preserve">F</t>
   </si>
   <si>
-    <t>Mobile</t>
+    <t xml:space="preserve">Mobile</t>
   </si>
   <si>
-    <t>VCT</t>
+    <t xml:space="preserve">VCT</t>
   </si>
   <si>
-    <t>Other community platform</t>
+    <t xml:space="preserve">Other community platform</t>
   </si>
   <si>
-    <t>Facility</t>
+    <t xml:space="preserve">Facility</t>
   </si>
   <si>
-    <t>STI</t>
+    <t xml:space="preserve">STI</t>
   </si>
   <si>
-    <t>Inpatient</t>
+    <t xml:space="preserve">Inpatient</t>
   </si>
   <si>
-    <t>Emergency</t>
+    <t xml:space="preserve">Emergency</t>
   </si>
   <si>
-    <t>TB</t>
+    <t xml:space="preserve">TB</t>
   </si>
   <si>
-    <t>VMMC</t>
+    <t xml:space="preserve">VMMC</t>
   </si>
   <si>
-    <t>PMTCT (ANC)</t>
+    <t xml:space="preserve">PMTCT (ANC)</t>
   </si>
   <si>
-    <t>Pediatric</t>
+    <t xml:space="preserve">Pediatric</t>
   </si>
   <si>
-    <t>&lt;5</t>
+    <t xml:space="preserve">&lt;5</t>
   </si>
   <si>
-    <t>Malnutrition</t>
+    <t xml:space="preserve">Malnutrition</t>
   </si>
   <si>
-    <t>Other PITC</t>
+    <t xml:space="preserve">Other PITC</t>
   </si>
   <si>
-    <t>HTS_SELF</t>
+    <t xml:space="preserve">HTS_SELF</t>
   </si>
   <si>
-    <t>Any</t>
+    <t xml:space="preserve">Any</t>
   </si>
   <si>
-    <t>Directly-assisted</t>
+    <t xml:space="preserve">Directly-assisted</t>
   </si>
   <si>
-    <t>Unassisted</t>
+    <t xml:space="preserve">Unassisted</t>
   </si>
   <si>
-    <t>Domain</t>
+    <t xml:space="preserve">Domain</t>
   </si>
   <si>
-    <t>Malawi MOH HTS</t>
+    <t xml:space="preserve">Malawi MOH HTS</t>
   </si>
   <si>
-    <t>PEPFAR MER 2.2</t>
+    <t xml:space="preserve">PEPFAR MER 2.2</t>
   </si>
   <si>
-    <t>Data Source</t>
+    <t xml:space="preserve">Data Source</t>
   </si>
   <si>
-    <t>Register attribute</t>
+    <t xml:space="preserve">Register attribute</t>
   </si>
   <si>
-    <t>Client record</t>
+    <t xml:space="preserve">Client record</t>
   </si>
   <si>
-    <t>Synthesis</t>
+    <t xml:space="preserve">Synthesis</t>
   </si>
   <si>
-    <t>Dimension</t>
+    <t xml:space="preserve">Dimension</t>
   </si>
   <si>
-    <t>Location Type</t>
+    <t xml:space="preserve">Location Type</t>
   </si>
   <si>
-    <t>Service Delivery Point</t>
+    <t xml:space="preserve">Service Delivery Point</t>
   </si>
   <si>
-    <t>Access Type</t>
+    <t xml:space="preserve">Access Type</t>
   </si>
   <si>
-    <t>Partner HIV Status</t>
+    <t xml:space="preserve">Partner HIV Status</t>
   </si>
   <si>
-    <t>Client Age</t>
+    <t xml:space="preserve">Client Age</t>
   </si>
   <si>
-    <t>HTS Setting</t>
+    <t xml:space="preserve">Client Gender</t>
   </si>
   <si>
-    <t>HTS Modality</t>
+    <t xml:space="preserve">HTS Setting</t>
   </si>
   <si>
-    <t>FRS/Index</t>
+    <t xml:space="preserve">HTS Modality</t>
   </si>
   <si>
-    <t>0-13Y</t>
+    <t xml:space="preserve">FRS/Index</t>
   </si>
   <si>
-    <t>Any other</t>
+    <t xml:space="preserve">0-13Y</t>
   </si>
   <si>
-    <t>Partner Positive</t>
+    <t xml:space="preserve">Any other</t>
   </si>
   <si>
-    <t>PITC</t>
+    <t xml:space="preserve">Partner Positive</t>
   </si>
   <si>
-    <t>VCT/Other</t>
+    <t xml:space="preserve">PITC</t>
   </si>
   <si>
-    <t>Other</t>
+    <t xml:space="preserve">VCT/Other</t>
   </si>
   <si>
-    <t>Health Facility</t>
+    <t xml:space="preserve">Health Facility</t>
   </si>
   <si>
-    <t>ANC</t>
+    <t xml:space="preserve">ANC</t>
   </si>
   <si>
-    <t>0-4Y</t>
+    <t xml:space="preserve">0-4Y</t>
   </si>
   <si>
-    <t>5Y+</t>
+    <t xml:space="preserve">5Y+</t>
   </si>
   <si>
-    <t>Maternity</t>
+    <t xml:space="preserve">Maternity</t>
   </si>
   <si>
-    <t>OPD</t>
+    <t xml:space="preserve">OPD</t>
   </si>
   <si>
-    <t>Stand-alone HTS Facility</t>
+    <t xml:space="preserve">Stand-alone HTS Facility</t>
   </si>
 </sst>
 </file>
@@ -300,7 +305,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="10">
@@ -478,8 +483,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Good" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Bad" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Bad" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -558,12 +563,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1457489878543"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3562753036437"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2793522267206"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.71255060728745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9622,26 +9627,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C76" activeCellId="0" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1457489878542"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.8542510121458"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.7125506072875"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.5748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>42</v>
       </c>
@@ -9652,12 +9657,13 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>45</v>
       </c>
@@ -9676,14 +9682,17 @@
       <c r="F2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>48</v>
+      <c r="G2" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>49</v>
       </c>
@@ -9708,8 +9717,11 @@
       <c r="H3" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
@@ -9717,22 +9729,25 @@
         <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>7</v>
       </c>
@@ -9740,22 +9755,25 @@
         <v>24</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>7</v>
       </c>
@@ -9763,22 +9781,25 @@
         <v>24</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
         <v>7</v>
       </c>
@@ -9786,7 +9807,7 @@
         <v>24</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>39</v>
@@ -9795,13 +9816,16 @@
         <v>39</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>7</v>
       </c>
@@ -9809,7 +9833,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>39</v>
@@ -9818,13 +9842,16 @@
         <v>39</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>7</v>
       </c>
@@ -9832,22 +9859,25 @@
         <v>63</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>7</v>
       </c>
@@ -9855,22 +9885,25 @@
         <v>63</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>7</v>
       </c>
@@ -9878,22 +9911,25 @@
         <v>63</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
         <v>7</v>
       </c>
@@ -9901,7 +9937,7 @@
         <v>63</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>39</v>
@@ -9910,13 +9946,16 @@
         <v>39</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="0" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>7</v>
       </c>
@@ -9924,7 +9963,7 @@
         <v>63</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>39</v>
@@ -9933,13 +9972,16 @@
         <v>39</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="H13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>64</v>
       </c>
@@ -9947,22 +9989,25 @@
         <v>65</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>64</v>
       </c>
@@ -9970,22 +10015,25 @@
         <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>64</v>
       </c>
@@ -9993,7 +10041,7 @@
         <v>65</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>60</v>
@@ -10002,13 +10050,16 @@
         <v>39</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
         <v>64</v>
       </c>
@@ -10016,22 +10067,25 @@
         <v>65</v>
       </c>
       <c r="D17" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="F17" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>64</v>
       </c>
@@ -10048,59 +10102,68 @@
         <v>39</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>64</v>
       </c>
@@ -10108,22 +10171,25 @@
         <v>29</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>64</v>
       </c>
@@ -10131,22 +10197,25 @@
         <v>29</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H22" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="0" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>64</v>
       </c>
@@ -10154,68 +10223,77 @@
         <v>29</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>64</v>
       </c>
@@ -10223,22 +10301,25 @@
         <v>36</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E26" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="G26" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
         <v>64</v>
       </c>
@@ -10246,22 +10327,25 @@
         <v>36</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>66</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
         <v>64</v>
       </c>
@@ -10269,22 +10353,25 @@
         <v>36</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F28" s="0" t="s">
         <v>67</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
         <v>64</v>
       </c>
@@ -10301,13 +10388,16 @@
         <v>66</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>64</v>
       </c>
@@ -10324,59 +10414,68 @@
         <v>67</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>68</v>
+        <v>36</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>64</v>
       </c>
@@ -10384,22 +10483,25 @@
         <v>68</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H33" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
         <v>64</v>
       </c>
@@ -10407,22 +10509,25 @@
         <v>68</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F34" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H34" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
         <v>64</v>
       </c>
@@ -10430,68 +10535,77 @@
         <v>68</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F35" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E36" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F37" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
         <v>64</v>
       </c>
@@ -10499,22 +10613,25 @@
         <v>69</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E38" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I38" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
         <v>64</v>
       </c>
@@ -10522,68 +10639,77 @@
         <v>69</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F39" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I39" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E40" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I40" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C41" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="E41" s="0" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F41" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I41" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>64</v>
       </c>
@@ -10591,22 +10717,25 @@
         <v>63</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H42" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>64</v>
       </c>
@@ -10614,22 +10743,25 @@
         <v>63</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F43" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H43" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I43" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>64</v>
       </c>
@@ -10637,68 +10769,77 @@
         <v>63</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F44" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I44" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E45" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I46" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
         <v>64</v>
       </c>
@@ -10706,22 +10847,25 @@
         <v>34</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E47" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F47" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F47" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="G47" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I47" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
         <v>64</v>
       </c>
@@ -10729,22 +10873,25 @@
         <v>34</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F48" s="0" t="s">
         <v>66</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H48" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I48" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
         <v>64</v>
       </c>
@@ -10752,22 +10899,25 @@
         <v>34</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F49" s="0" t="s">
         <v>67</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H49" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I49" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>64</v>
       </c>
@@ -10784,13 +10934,16 @@
         <v>66</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
         <v>64</v>
       </c>
@@ -10807,59 +10960,68 @@
         <v>67</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I51" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E52" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>64</v>
       </c>
@@ -10867,22 +11029,25 @@
         <v>28</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H54" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I54" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
         <v>64</v>
       </c>
@@ -10890,22 +11055,25 @@
         <v>28</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F55" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H55" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I55" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
         <v>64</v>
       </c>
@@ -10913,68 +11081,77 @@
         <v>28</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F56" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E57" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F58" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
         <v>64</v>
       </c>
@@ -10982,22 +11159,25 @@
         <v>31</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H59" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I59" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
         <v>64</v>
       </c>
@@ -11005,22 +11185,25 @@
         <v>31</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F60" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H60" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I60" s="0" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
         <v>64</v>
       </c>
@@ -11028,68 +11211,77 @@
         <v>31</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F61" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E62" s="0" t="s">
         <v>39</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
         <v>64</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="F63" s="0" t="s">
         <v>39</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
         <v>64</v>
       </c>
@@ -11097,22 +11289,25 @@
         <v>32</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H64" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
         <v>64</v>
       </c>
@@ -11120,22 +11315,25 @@
         <v>32</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H65" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I65" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
         <v>64</v>
       </c>
@@ -11143,114 +11341,129 @@
         <v>32</v>
       </c>
       <c r="D66" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D68" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E66" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F66" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G66" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H66" s="0" t="s">
+      <c r="E68" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F68" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H68" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I68" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E70" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F70" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G70" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H70" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I70" s="0" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E67" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F67" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G67" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H67" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E68" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F68" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G68" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H68" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E69" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="F69" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G69" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H69" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E70" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F70" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G70" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H70" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
         <v>70</v>
       </c>
@@ -11258,25 +11471,132 @@
         <v>63</v>
       </c>
       <c r="D71" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E71" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F71" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G71" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H72" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H73" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D74" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E71" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F71" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G71" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H71" s="0" t="s">
+      <c r="E74" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H74" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I75" s="0" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Updated mapping for indicator mapping in PEPFAR data synthesis
</commit_message>
<xml_diff>
--- a/designs/MER2.2 HTS indicator review, version 2.xlsx
+++ b/designs/MER2.2 HTS indicator review, version 2.xlsx
@@ -51,32 +51,6 @@
           <t xml:space="preserve">FRS are issued for 2 groups in the national program:
 1) Client has partner with unknown HIV status, regardless of HIV status of the client him/herself
 2) Client is HIV positive and has children under 13 with unknown status</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Andreas Jahn:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Emergency: Includes persons tested or seen in a designated emergency department or ward for the immediate care and treatment of an unforeseen illness or injury.</t>
         </r>
       </text>
     </comment>
@@ -9629,8 +9603,8 @@
   </sheetPr>
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C76" activeCellId="0" sqref="C76"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
More fixes on PEPFAR report missing data
</commit_message>
<xml_diff>
--- a/designs/MER2.2 HTS indicator review, version 2.xlsx
+++ b/designs/MER2.2 HTS indicator review, version 2.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MER2.2_HTS_TST+HTS_SELF" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="MOH_MER2.2_mapping" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'MOH_MER2.2_mapping'!$D$2:$D$71</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'MOH_MER2.2_mapping'!$H:$H</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'MOH_MER2.2_mapping'!$D$2:$D$71</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -342,13 +343,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="16"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -358,6 +352,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -378,18 +379,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -420,7 +415,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -444,10 +439,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -468,36 +460,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Good" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Bad" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -535,7 +526,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFC6EFCE"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -581,7 +572,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1417004048583"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.89068825910931"/>
@@ -9641,25 +9632,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G76" activeCellId="0" sqref="G76"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -9705,7 +9696,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>49</v>
       </c>
@@ -9731,7 +9722,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
@@ -9754,7 +9745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
         <v>7</v>
       </c>
@@ -9777,7 +9768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>7</v>
       </c>
@@ -9823,7 +9814,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>7</v>
       </c>
@@ -9846,7 +9837,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
         <v>7</v>
       </c>
@@ -9869,7 +9860,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
         <v>7</v>
       </c>
@@ -9892,7 +9883,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
         <v>7</v>
       </c>
@@ -9938,7 +9929,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
         <v>7</v>
       </c>
@@ -9961,7 +9952,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
         <v>64</v>
       </c>
@@ -9984,7 +9975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
         <v>64</v>
       </c>
@@ -10007,7 +9998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
         <v>64</v>
       </c>
@@ -10053,7 +10044,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
         <v>64</v>
       </c>
@@ -10076,7 +10067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
         <v>64</v>
       </c>
@@ -10099,7 +10090,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
         <v>64</v>
       </c>
@@ -10122,7 +10113,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
         <v>64</v>
       </c>
@@ -10168,7 +10159,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
         <v>64</v>
       </c>
@@ -10191,7 +10182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>64</v>
       </c>
@@ -10214,7 +10205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
         <v>64</v>
       </c>
@@ -10237,7 +10228,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>64</v>
       </c>
@@ -10306,7 +10297,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
         <v>64</v>
       </c>
@@ -10329,7 +10320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
         <v>64</v>
       </c>
@@ -10352,7 +10343,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
         <v>64</v>
       </c>
@@ -10375,7 +10366,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
         <v>64</v>
       </c>
@@ -10398,7 +10389,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
         <v>64</v>
       </c>
@@ -10444,7 +10435,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
         <v>64</v>
       </c>
@@ -10467,7 +10458,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
         <v>64</v>
       </c>
@@ -10490,7 +10481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
         <v>64</v>
       </c>
@@ -10536,7 +10527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
         <v>64</v>
       </c>
@@ -10559,7 +10550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>64</v>
       </c>
@@ -10582,7 +10573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
         <v>64</v>
       </c>
@@ -10605,7 +10596,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>64</v>
       </c>
@@ -10651,7 +10642,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>64</v>
       </c>
@@ -10674,7 +10665,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>64</v>
       </c>
@@ -10697,7 +10688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>64</v>
       </c>
@@ -10720,7 +10711,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
         <v>64</v>
       </c>
@@ -10789,7 +10780,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
         <v>64</v>
       </c>
@@ -10812,7 +10803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
         <v>64</v>
       </c>
@@ -10835,7 +10826,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
         <v>64</v>
       </c>
@@ -10858,7 +10849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
         <v>64</v>
       </c>
@@ -10881,7 +10872,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>64</v>
       </c>
@@ -10927,7 +10918,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
         <v>64</v>
       </c>
@@ -10950,7 +10941,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
         <v>64</v>
       </c>
@@ -10973,7 +10964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
         <v>64</v>
       </c>
@@ -10996,7 +10987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
         <v>64</v>
       </c>
@@ -11042,7 +11033,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
         <v>64</v>
       </c>
@@ -11065,7 +11056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
         <v>64</v>
       </c>
@@ -11088,7 +11079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
         <v>64</v>
       </c>
@@ -11111,7 +11102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
         <v>64</v>
       </c>
@@ -11157,7 +11148,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
         <v>64</v>
       </c>
@@ -11180,7 +11171,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
         <v>70</v>
       </c>
@@ -11203,7 +11194,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
         <v>70</v>
       </c>
@@ -11226,7 +11217,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
         <v>70</v>
       </c>
@@ -11272,7 +11263,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
         <v>70</v>
       </c>
@@ -11296,13 +11287,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D2:D71">
-    <filterColumn colId="0">
-      <customFilters and="true">
-        <customFilter operator="equal" val="PITC"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="H:H"/>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>